<commit_message>
Excell de atributos y objetos.
</commit_message>
<xml_diff>
--- a/Archivos_Excel_Matrices/Objetos y atributos.xlsx
+++ b/Archivos_Excel_Matrices/Objetos y atributos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo\Dropbox\Gente\Víctor-Memo\TESIS!!!\Diseño\Nueva distribucion de brete\5. Operaciones\Programación de Rutas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -17,9 +12,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$1:$F$28</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>asociado</t>
   </si>
@@ -249,13 +244,16 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,9 +346,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -362,6 +357,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,7 +456,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,23 +633,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E25"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
@@ -659,28 +657,28 @@
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -699,8 +697,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -719,8 +717,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+    <row r="4" spans="1:6" ht="90">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -739,8 +737,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+    <row r="5" spans="1:6" ht="75">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -759,8 +757,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+    <row r="6" spans="1:6">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -779,8 +777,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+    <row r="7" spans="1:6">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -799,8 +797,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -819,8 +817,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -839,8 +837,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -859,8 +857,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -879,8 +877,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+    <row r="12" spans="1:6" ht="45">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -899,8 +897,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+    <row r="13" spans="1:6">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -912,15 +910,15 @@
       <c r="D13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="11" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+    <row r="14" spans="1:6">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -932,13 +930,13 @@
       <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -955,8 +953,8 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -975,8 +973,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -995,8 +993,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+    <row r="18" spans="1:6">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1015,8 +1013,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+    <row r="19" spans="1:6">
+      <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1035,8 +1033,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+    <row r="20" spans="1:6">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1055,8 +1053,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+    <row r="21" spans="1:6">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1075,8 +1073,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+    <row r="22" spans="1:6" ht="38.25">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1095,8 +1093,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+    <row r="23" spans="1:6">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1108,15 +1106,15 @@
       <c r="D23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="11" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+    <row r="24" spans="1:6">
+      <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1128,13 +1126,13 @@
       <c r="D24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+    <row r="25" spans="1:6" ht="30">
+      <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1146,13 +1144,13 @@
       <c r="D25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+    <row r="26" spans="1:6">
+      <c r="A26" s="8">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1171,8 +1169,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+    <row r="27" spans="1:6" ht="38.25">
+      <c r="A27" s="8">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1191,8 +1189,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+    <row r="28" spans="1:6" ht="25.5">
+      <c r="A28" s="8">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1209,6 +1207,11 @@
       </c>
       <c r="F28" s="1" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>